<commit_message>
actualización de audios y cuentos
</commit_message>
<xml_diff>
--- a/resultados_sistemas/cuentos_segundo_experimento/Resumen_resultados.xlsx
+++ b/resultados_sistemas/cuentos_segundo_experimento/Resumen_resultados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Cuentos\Resultados_sistema\data_aleatoria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7d8153ad8b51f3b/UAEMex/Period2024A/TESIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93645FCE-8F03-4651-B53B-A9202EEDEB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="442" documentId="8_{07CE2F0D-33F9-47A1-A8B1-0493600B9132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1BDBEC9-D3BC-4A9E-A553-687B5B5D2198}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A792917-A682-4AF0-A5E9-758AF4ACFB26}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{9A792917-A682-4AF0-A5E9-758AF4ACFB26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,6 +77,9 @@
     <t>Cuidado del medio ambiente</t>
   </si>
   <si>
+    <t>Diego, Carlos, Emiliano</t>
+  </si>
+  <si>
     <t>Tema</t>
   </si>
   <si>
@@ -186,9 +189,6 @@
   </si>
   <si>
     <t>Fernanda, diego, isabella</t>
-  </si>
-  <si>
-    <t>Diego, Carlos, Emilio</t>
   </si>
 </sst>
 </file>
@@ -210,12 +210,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -238,6 +244,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -576,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4EFE13A-73D7-4306-9CBD-1D69CA013000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,6 +596,7 @@
     <col min="4" max="4" width="27.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -601,16 +610,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
         <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -621,19 +630,19 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2">
-        <v>13.6067774295806</v>
+        <v>22.1903717517852</v>
       </c>
       <c r="G2" s="2">
-        <v>5.4166666666666669E-2</v>
+        <v>0.10208333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -644,13 +653,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3">
         <v>10.7646219730377</v>
@@ -667,13 +676,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4">
         <v>10.738414764404199</v>
@@ -690,13 +699,13 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F5" s="5">
         <v>11.747601270675601</v>
@@ -713,13 +722,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>8.2069077491760201</v>
@@ -736,13 +745,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7">
         <v>12.314956903457601</v>
@@ -759,13 +768,13 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8">
         <v>10.1476078033447</v>
@@ -782,13 +791,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F9">
         <v>7.8123278617858798</v>
@@ -805,13 +814,13 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F10">
         <v>17.442980766296301</v>
@@ -828,13 +837,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11">
         <v>13.3438639640808</v>
@@ -851,13 +860,13 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12">
         <v>15.3553721904754</v>
@@ -874,13 +883,13 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F13">
         <v>9.2956490516662598</v>
@@ -897,13 +906,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F14" s="5">
         <v>11.255607366561801</v>
@@ -912,26 +921,26 @@
         <v>4.3749999999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:7" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15">
+      <c r="E15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="7">
         <v>8.2540457248687709</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="8">
         <v>3.6111111111111108E-2</v>
       </c>
     </row>
@@ -943,13 +952,13 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16">
         <v>11.1978201866149</v>
@@ -966,13 +975,13 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F17">
         <v>8.2607946395874006</v>
@@ -989,13 +998,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F18" s="3">
         <v>11.4256083965301</v>
@@ -1012,13 +1021,13 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>9.4364950656890798</v>
@@ -1035,22 +1044,22 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F20">
-        <v>8.8796331882476807</v>
+        <v>13.457445859909001</v>
       </c>
       <c r="G20" s="2">
-        <v>3.4027777777777775E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>5.347222222222222E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1058,19 +1067,19 @@
         <v>3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F21" s="5">
-        <v>11.2546832561492</v>
+        <v>19.1971867084503</v>
       </c>
       <c r="G21" s="6">
-        <v>4.027777777777778E-2</v>
+        <v>7.9861111111111105E-2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1081,19 +1090,19 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F22">
-        <v>10.476708412170399</v>
+        <v>19.0394718647003</v>
       </c>
       <c r="G22" s="2">
-        <v>3.888888888888889E-2</v>
+        <v>8.819444444444445E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1104,13 +1113,13 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F23">
         <v>13.138364791870099</v>
@@ -1127,13 +1136,13 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F24">
         <v>13.140708208084099</v>
@@ -1142,26 +1151,26 @@
         <v>4.9305555555555554E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25">
+      <c r="E25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="7">
         <v>15.3344166278839</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="8">
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
@@ -1173,19 +1182,19 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F26">
-        <v>11.210126399993801</v>
+        <v>25.3284590244293</v>
       </c>
       <c r="G26" s="2">
-        <v>4.3749999999999997E-2</v>
+        <v>7.6388888888888895E-2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1196,41 +1205,41 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F27">
         <v>10.6906495094299</v>
       </c>
       <c r="G27" s="2">
-        <v>4.027777777777778E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28">
+      <c r="E28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="7">
         <v>11.487216711044301</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="8">
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
@@ -1242,13 +1251,13 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F29">
         <v>9.4463763236999494</v>
@@ -1265,13 +1274,13 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F30">
         <v>10.568477630615201</v>
@@ -1288,19 +1297,19 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F31">
-        <v>8.5530970096588099</v>
+        <v>19.146659374237</v>
       </c>
       <c r="G31" s="2">
-        <v>2.9861111111111113E-2</v>
+        <v>8.1250000000000003E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>